<commit_message>
Changed hydgn/HPEbP electrolysis efficiency values to 0.6 in 2030 and to 0.7 in 2050 for agora industry analysis to match their BAU
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HPEbP/Hydgn Production Eff by Pathway.xlsx
+++ b/InputData/hydgn/HPEbP/Hydgn Production Eff by Pathway.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\hydgn\HPEbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-eu\InputData\hydgn\HPEbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EC745A-4E58-4AFD-ACA2-B7C1EAEE38C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25820" windowHeight="11970"/>
+    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="IEA Data" sheetId="3" r:id="rId2"/>
-    <sheet name="HPEbP" sheetId="2" r:id="rId3"/>
+    <sheet name="prev_electrolysis_values" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="HPEbP" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>HPEbP Hydrogen Production Efficiency by Pathway</t>
   </si>
@@ -164,12 +176,18 @@
   </si>
   <si>
     <t>Appendix D (biomass), Appendix H (natural gas), Appendix I (electrolysis), and Appendix J (coal)</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>formulas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -547,10 +565,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -684,8 +702,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -693,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -978,14 +996,504 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B33DF6D-EC1F-4D31-AF58-E018728E369A}">
+  <dimension ref="A1:AI6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C2">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="E2">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G2">
+        <v>2022</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I2">
+        <v>2024</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2025</v>
+      </c>
+      <c r="K2">
+        <v>2026</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2027</v>
+      </c>
+      <c r="M2">
+        <v>2028</v>
+      </c>
+      <c r="N2" s="5">
+        <v>2029</v>
+      </c>
+      <c r="O2">
+        <v>2030</v>
+      </c>
+      <c r="P2" s="14">
+        <v>2031</v>
+      </c>
+      <c r="Q2">
+        <v>2032</v>
+      </c>
+      <c r="R2" s="5">
+        <v>2033</v>
+      </c>
+      <c r="S2">
+        <v>2034</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2035</v>
+      </c>
+      <c r="U2">
+        <v>2036</v>
+      </c>
+      <c r="V2" s="5">
+        <v>2037</v>
+      </c>
+      <c r="W2">
+        <v>2038</v>
+      </c>
+      <c r="X2" s="5">
+        <v>2039</v>
+      </c>
+      <c r="Y2">
+        <v>2040</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>2041</v>
+      </c>
+      <c r="AA2">
+        <v>2042</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>2043</v>
+      </c>
+      <c r="AC2">
+        <v>2044</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>2045</v>
+      </c>
+      <c r="AE2">
+        <v>2046</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>2047</v>
+      </c>
+      <c r="AG2">
+        <v>2048</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>2049</v>
+      </c>
+      <c r="AI2">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.67045454545454541</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.6743453210151954</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.67825867548826535</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.682194739903489</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.68615364605099072</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.69013552648569809</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.69414051453178016</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.69816874428711162</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.70222035062776267</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.70629546921251507</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.71039423648740441</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.71451678969028842</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.71866326685544257</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0.72283380681818132</v>
+      </c>
+      <c r="P3" s="13">
+        <v>0.7253666557451437</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>0.72790837991234292</v>
+      </c>
+      <c r="R3" s="12">
+        <v>0.73045901041910288</v>
+      </c>
+      <c r="S3" s="12">
+        <v>0.73301857847372121</v>
+      </c>
+      <c r="T3" s="12">
+        <v>0.73558711539385124</v>
+      </c>
+      <c r="U3" s="12">
+        <v>0.73816465260688491</v>
+      </c>
+      <c r="V3" s="12">
+        <v>0.74075122165033747</v>
+      </c>
+      <c r="W3" s="12">
+        <v>0.74334685417223334</v>
+      </c>
+      <c r="X3" s="12">
+        <v>0.74595158193149347</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>0.74856543679832355</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>0.7511884507546045</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>0.75382065589428315</v>
+      </c>
+      <c r="AB3" s="12">
+        <v>0.7564620844237655</v>
+      </c>
+      <c r="AC3" s="12">
+        <v>0.75911276866231048</v>
+      </c>
+      <c r="AD3" s="12">
+        <v>0.76177274104242554</v>
+      </c>
+      <c r="AE3" s="12">
+        <v>0.76444203411026324</v>
+      </c>
+      <c r="AF3" s="12">
+        <v>0.76712068052601967</v>
+      </c>
+      <c r="AG3" s="12">
+        <v>0.76980871306433407</v>
+      </c>
+      <c r="AH3" s="12">
+        <v>0.77250616461468979</v>
+      </c>
+      <c r="AI3" s="12">
+        <v>0.77521306818181679</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2019</v>
+      </c>
+      <c r="E5">
+        <v>2020</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G5">
+        <v>2022</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I5">
+        <v>2024</v>
+      </c>
+      <c r="J5" s="5">
+        <v>2025</v>
+      </c>
+      <c r="K5">
+        <v>2026</v>
+      </c>
+      <c r="L5" s="5">
+        <v>2027</v>
+      </c>
+      <c r="M5">
+        <v>2028</v>
+      </c>
+      <c r="N5" s="5">
+        <v>2029</v>
+      </c>
+      <c r="O5">
+        <v>2030</v>
+      </c>
+      <c r="P5" s="14">
+        <v>2031</v>
+      </c>
+      <c r="Q5">
+        <v>2032</v>
+      </c>
+      <c r="R5" s="5">
+        <v>2033</v>
+      </c>
+      <c r="S5">
+        <v>2034</v>
+      </c>
+      <c r="T5" s="5">
+        <v>2035</v>
+      </c>
+      <c r="U5">
+        <v>2036</v>
+      </c>
+      <c r="V5" s="5">
+        <v>2037</v>
+      </c>
+      <c r="W5">
+        <v>2038</v>
+      </c>
+      <c r="X5" s="5">
+        <v>2039</v>
+      </c>
+      <c r="Y5">
+        <v>2040</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>2041</v>
+      </c>
+      <c r="AA5">
+        <v>2042</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>2043</v>
+      </c>
+      <c r="AC5">
+        <v>2044</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>2045</v>
+      </c>
+      <c r="AE5">
+        <v>2046</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>2047</v>
+      </c>
+      <c r="AG5">
+        <v>2048</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>2049</v>
+      </c>
+      <c r="AI5">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <f>118/176</f>
+        <v>0.67045454545454541</v>
+      </c>
+      <c r="C6" s="6">
+        <f>B6*'IEA Data'!$D$18</f>
+        <v>0.6743453210151954</v>
+      </c>
+      <c r="D6" s="6">
+        <f>C6*'IEA Data'!$D$18</f>
+        <v>0.67825867548826535</v>
+      </c>
+      <c r="E6" s="6">
+        <f>D6*'IEA Data'!$D$18</f>
+        <v>0.682194739903489</v>
+      </c>
+      <c r="F6" s="6">
+        <f>E6*'IEA Data'!$D$18</f>
+        <v>0.68615364605099072</v>
+      </c>
+      <c r="G6" s="6">
+        <f>F6*'IEA Data'!$D$18</f>
+        <v>0.69013552648569809</v>
+      </c>
+      <c r="H6" s="6">
+        <f>G6*'IEA Data'!$D$18</f>
+        <v>0.69414051453178016</v>
+      </c>
+      <c r="I6" s="6">
+        <f>H6*'IEA Data'!$D$18</f>
+        <v>0.69816874428711162</v>
+      </c>
+      <c r="J6" s="6">
+        <f>I6*'IEA Data'!$D$18</f>
+        <v>0.70222035062776267</v>
+      </c>
+      <c r="K6" s="6">
+        <f>J6*'IEA Data'!$D$18</f>
+        <v>0.70629546921251507</v>
+      </c>
+      <c r="L6" s="6">
+        <f>K6*'IEA Data'!$D$18</f>
+        <v>0.71039423648740441</v>
+      </c>
+      <c r="M6" s="6">
+        <f>L6*'IEA Data'!$D$18</f>
+        <v>0.71451678969028842</v>
+      </c>
+      <c r="N6" s="6">
+        <f>M6*'IEA Data'!$D$18</f>
+        <v>0.71866326685544257</v>
+      </c>
+      <c r="O6" s="6">
+        <f>N6*'IEA Data'!$D$18</f>
+        <v>0.72283380681818132</v>
+      </c>
+      <c r="P6" s="13">
+        <f>O6*'IEA Data'!$E$18</f>
+        <v>0.7253666557451437</v>
+      </c>
+      <c r="Q6" s="12">
+        <f>P6*'IEA Data'!$E$18</f>
+        <v>0.72790837991234292</v>
+      </c>
+      <c r="R6" s="12">
+        <f>Q6*'IEA Data'!$E$18</f>
+        <v>0.73045901041910288</v>
+      </c>
+      <c r="S6" s="12">
+        <f>R6*'IEA Data'!$E$18</f>
+        <v>0.73301857847372121</v>
+      </c>
+      <c r="T6" s="12">
+        <f>S6*'IEA Data'!$E$18</f>
+        <v>0.73558711539385124</v>
+      </c>
+      <c r="U6" s="12">
+        <f>T6*'IEA Data'!$E$18</f>
+        <v>0.73816465260688491</v>
+      </c>
+      <c r="V6" s="12">
+        <f>U6*'IEA Data'!$E$18</f>
+        <v>0.74075122165033747</v>
+      </c>
+      <c r="W6" s="12">
+        <f>V6*'IEA Data'!$E$18</f>
+        <v>0.74334685417223334</v>
+      </c>
+      <c r="X6" s="12">
+        <f>W6*'IEA Data'!$E$18</f>
+        <v>0.74595158193149347</v>
+      </c>
+      <c r="Y6" s="12">
+        <f>X6*'IEA Data'!$E$18</f>
+        <v>0.74856543679832355</v>
+      </c>
+      <c r="Z6" s="12">
+        <f>Y6*'IEA Data'!$E$18</f>
+        <v>0.7511884507546045</v>
+      </c>
+      <c r="AA6" s="12">
+        <f>Z6*'IEA Data'!$E$18</f>
+        <v>0.75382065589428315</v>
+      </c>
+      <c r="AB6" s="12">
+        <f>AA6*'IEA Data'!$E$18</f>
+        <v>0.7564620844237655</v>
+      </c>
+      <c r="AC6" s="12">
+        <f>AB6*'IEA Data'!$E$18</f>
+        <v>0.75911276866231048</v>
+      </c>
+      <c r="AD6" s="12">
+        <f>AC6*'IEA Data'!$E$18</f>
+        <v>0.76177274104242554</v>
+      </c>
+      <c r="AE6" s="12">
+        <f>AD6*'IEA Data'!$E$18</f>
+        <v>0.76444203411026324</v>
+      </c>
+      <c r="AF6" s="12">
+        <f>AE6*'IEA Data'!$E$18</f>
+        <v>0.76712068052601967</v>
+      </c>
+      <c r="AG6" s="12">
+        <f>AF6*'IEA Data'!$E$18</f>
+        <v>0.76980871306433407</v>
+      </c>
+      <c r="AH6" s="12">
+        <f>AG6*'IEA Data'!$E$18</f>
+        <v>0.77250616461468979</v>
+      </c>
+      <c r="AI6" s="12">
+        <f>AH6*'IEA Data'!$E$18</f>
+        <v>0.77521306818181679</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H17:H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1106,140 +1614,140 @@
         <v>2</v>
       </c>
       <c r="B2" s="6">
-        <f>118/176</f>
-        <v>0.67045454545454541</v>
+        <f>0.6</f>
+        <v>0.6</v>
       </c>
       <c r="C2" s="6">
-        <f>B2*'IEA Data'!$D$18</f>
-        <v>0.6743453210151954</v>
+        <f t="shared" ref="C2:O2" si="0">0.6</f>
+        <v>0.6</v>
       </c>
       <c r="D2" s="6">
-        <f>C2*'IEA Data'!$D$18</f>
-        <v>0.67825867548826535</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="E2" s="6">
-        <f>D2*'IEA Data'!$D$18</f>
-        <v>0.682194739903489</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="F2" s="6">
-        <f>E2*'IEA Data'!$D$18</f>
-        <v>0.68615364605099072</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="G2" s="6">
-        <f>F2*'IEA Data'!$D$18</f>
-        <v>0.69013552648569809</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="H2" s="6">
-        <f>G2*'IEA Data'!$D$18</f>
-        <v>0.69414051453178016</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="I2" s="6">
-        <f>H2*'IEA Data'!$D$18</f>
-        <v>0.69816874428711162</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="J2" s="6">
-        <f>I2*'IEA Data'!$D$18</f>
-        <v>0.70222035062776267</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="K2" s="6">
-        <f>J2*'IEA Data'!$D$18</f>
-        <v>0.70629546921251507</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="L2" s="6">
-        <f>K2*'IEA Data'!$D$18</f>
-        <v>0.71039423648740441</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="M2" s="6">
-        <f>L2*'IEA Data'!$D$18</f>
-        <v>0.71451678969028842</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="N2" s="6">
-        <f>M2*'IEA Data'!$D$18</f>
-        <v>0.71866326685544257</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="O2" s="6">
-        <f>N2*'IEA Data'!$D$18</f>
-        <v>0.72283380681818132</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="P2" s="13">
-        <f>O2*'IEA Data'!$E$18</f>
-        <v>0.7253666557451437</v>
+        <f>O2+(($AI$2-$O$2)/COUNT($P$1:$AI$1))</f>
+        <v>0.60499999999999998</v>
       </c>
       <c r="Q2" s="12">
-        <f>P2*'IEA Data'!$E$18</f>
-        <v>0.72790837991234292</v>
+        <f t="shared" ref="Q2:AH2" si="1">P2+(($AI$2-$O$2)/COUNT($P$1:$AI$1))</f>
+        <v>0.61</v>
       </c>
       <c r="R2" s="12">
-        <f>Q2*'IEA Data'!$E$18</f>
-        <v>0.73045901041910288</v>
+        <f t="shared" si="1"/>
+        <v>0.61499999999999999</v>
       </c>
       <c r="S2" s="12">
-        <f>R2*'IEA Data'!$E$18</f>
-        <v>0.73301857847372121</v>
+        <f t="shared" si="1"/>
+        <v>0.62</v>
       </c>
       <c r="T2" s="12">
-        <f>S2*'IEA Data'!$E$18</f>
-        <v>0.73558711539385124</v>
+        <f t="shared" si="1"/>
+        <v>0.625</v>
       </c>
       <c r="U2" s="12">
-        <f>T2*'IEA Data'!$E$18</f>
-        <v>0.73816465260688491</v>
+        <f t="shared" si="1"/>
+        <v>0.63</v>
       </c>
       <c r="V2" s="12">
-        <f>U2*'IEA Data'!$E$18</f>
-        <v>0.74075122165033747</v>
+        <f t="shared" si="1"/>
+        <v>0.63500000000000001</v>
       </c>
       <c r="W2" s="12">
-        <f>V2*'IEA Data'!$E$18</f>
-        <v>0.74334685417223334</v>
+        <f t="shared" si="1"/>
+        <v>0.64</v>
       </c>
       <c r="X2" s="12">
-        <f>W2*'IEA Data'!$E$18</f>
-        <v>0.74595158193149347</v>
+        <f t="shared" si="1"/>
+        <v>0.64500000000000002</v>
       </c>
       <c r="Y2" s="12">
-        <f>X2*'IEA Data'!$E$18</f>
-        <v>0.74856543679832355</v>
+        <f t="shared" si="1"/>
+        <v>0.65</v>
       </c>
       <c r="Z2" s="12">
-        <f>Y2*'IEA Data'!$E$18</f>
-        <v>0.7511884507546045</v>
+        <f t="shared" si="1"/>
+        <v>0.65500000000000003</v>
       </c>
       <c r="AA2" s="12">
-        <f>Z2*'IEA Data'!$E$18</f>
-        <v>0.75382065589428315</v>
+        <f t="shared" si="1"/>
+        <v>0.66</v>
       </c>
       <c r="AB2" s="12">
-        <f>AA2*'IEA Data'!$E$18</f>
-        <v>0.7564620844237655</v>
+        <f t="shared" si="1"/>
+        <v>0.66500000000000004</v>
       </c>
       <c r="AC2" s="12">
-        <f>AB2*'IEA Data'!$E$18</f>
-        <v>0.75911276866231048</v>
+        <f t="shared" si="1"/>
+        <v>0.67</v>
       </c>
       <c r="AD2" s="12">
-        <f>AC2*'IEA Data'!$E$18</f>
-        <v>0.76177274104242554</v>
+        <f t="shared" si="1"/>
+        <v>0.67500000000000004</v>
       </c>
       <c r="AE2" s="12">
-        <f>AD2*'IEA Data'!$E$18</f>
-        <v>0.76444203411026324</v>
+        <f t="shared" si="1"/>
+        <v>0.68</v>
       </c>
       <c r="AF2" s="12">
-        <f>AE2*'IEA Data'!$E$18</f>
-        <v>0.76712068052601967</v>
+        <f t="shared" si="1"/>
+        <v>0.68500000000000005</v>
       </c>
       <c r="AG2" s="12">
-        <f>AF2*'IEA Data'!$E$18</f>
-        <v>0.76980871306433407</v>
+        <f t="shared" si="1"/>
+        <v>0.69000000000000006</v>
       </c>
       <c r="AH2" s="12">
-        <f>AG2*'IEA Data'!$E$18</f>
-        <v>0.77250616461468979</v>
+        <f t="shared" si="1"/>
+        <v>0.69500000000000006</v>
       </c>
       <c r="AI2" s="12">
-        <f>AH2*'IEA Data'!$E$18</f>
-        <v>0.77521306818181679</v>
+        <f>0.7</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
@@ -1255,51 +1763,51 @@
         <v>0.56190476190476191</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:O3" si="0">C3</f>
+        <f t="shared" ref="D3:O3" si="2">C3</f>
         <v>0.56190476190476191</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="H3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="I3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="J3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="K3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="L3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="M3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="N3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="O3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="P3" s="13">
@@ -1307,79 +1815,79 @@
         <v>0.56190476190476191</v>
       </c>
       <c r="Q3" s="12">
-        <f t="shared" ref="Q3:AI3" si="1">P3</f>
+        <f t="shared" ref="Q3:AI3" si="3">P3</f>
         <v>0.56190476190476191</v>
       </c>
       <c r="R3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="S3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="T3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="U3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="V3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="W3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="X3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="Y3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="Z3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AA3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AB3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AC3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AD3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AE3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AF3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AG3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AH3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
       <c r="AI3" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56190476190476191</v>
       </c>
     </row>
@@ -1392,135 +1900,135 @@
         <v>0.57004830917874394</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:P6" si="2">B4</f>
+        <f t="shared" ref="C4:P6" si="4">B4</f>
         <v>0.57004830917874394</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="E4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="H4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="I4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="K4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="M4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="N4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="O4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="P4" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="Q4" s="12">
-        <f t="shared" ref="Q4:AI4" si="3">P4</f>
+        <f t="shared" ref="Q4:AI4" si="5">P4</f>
         <v>0.57004830917874394</v>
       </c>
       <c r="R4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="S4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="T4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="U4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="V4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="W4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="X4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="Y4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="Z4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AA4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AB4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AC4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AD4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AE4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AF4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AG4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AH4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
       <c r="AI4" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57004830917874394</v>
       </c>
     </row>
@@ -1533,135 +2041,135 @@
         <v>0.46274509803921571</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="H5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="K5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="N5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="O5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="P5" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="Q5" s="12">
-        <f t="shared" ref="Q5:AI5" si="4">P5</f>
+        <f t="shared" ref="Q5:AI5" si="6">P5</f>
         <v>0.46274509803921571</v>
       </c>
       <c r="R5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="T5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="U5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="V5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="X5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="Y5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="Z5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AB5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AC5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AD5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AE5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AF5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AG5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AH5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
       <c r="AI5" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46274509803921571</v>
       </c>
     </row>
@@ -1673,135 +2181,135 @@
         <v>0</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P6" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q6" s="12">
-        <f t="shared" ref="Q6:AI6" si="5">P6</f>
+        <f t="shared" ref="Q6:AI6" si="7">P6</f>
         <v>0</v>
       </c>
       <c r="R6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AE6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI6" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3.3.1.1 --> 3.4.0 update hydgn/HPEbP
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HPEbP/Hydgn Production Eff by Pathway.xlsx
+++ b/InputData/hydgn/HPEbP/Hydgn Production Eff by Pathway.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\hydgn\HPEbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\hydgn\HPEbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{495E05C4-D094-4446-BF1F-E6161A1DFE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25820" windowHeight="11970"/>
+    <workbookView xWindow="36015" yWindow="2070" windowWidth="17985" windowHeight="12525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="IEA Data" sheetId="3" r:id="rId2"/>
     <sheet name="HPEbP" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -169,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -243,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -262,7 +274,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -547,11 +558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,8 +695,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -693,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,14 +989,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H17:H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,7 +1051,7 @@
       <c r="O1">
         <v>2030</v>
       </c>
-      <c r="P1" s="14">
+      <c r="P1" s="13">
         <v>2031</v>
       </c>
       <c r="Q1">
@@ -1161,83 +1172,83 @@
         <f>N2*'IEA Data'!$D$18</f>
         <v>0.72283380681818132</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="12">
         <f>O2*'IEA Data'!$E$18</f>
         <v>0.7253666557451437</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="6">
         <f>P2*'IEA Data'!$E$18</f>
         <v>0.72790837991234292</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="6">
         <f>Q2*'IEA Data'!$E$18</f>
         <v>0.73045901041910288</v>
       </c>
-      <c r="S2" s="12">
+      <c r="S2" s="6">
         <f>R2*'IEA Data'!$E$18</f>
         <v>0.73301857847372121</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="6">
         <f>S2*'IEA Data'!$E$18</f>
         <v>0.73558711539385124</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="6">
         <f>T2*'IEA Data'!$E$18</f>
         <v>0.73816465260688491</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="6">
         <f>U2*'IEA Data'!$E$18</f>
         <v>0.74075122165033747</v>
       </c>
-      <c r="W2" s="12">
+      <c r="W2" s="6">
         <f>V2*'IEA Data'!$E$18</f>
         <v>0.74334685417223334</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="6">
         <f>W2*'IEA Data'!$E$18</f>
         <v>0.74595158193149347</v>
       </c>
-      <c r="Y2" s="12">
+      <c r="Y2" s="6">
         <f>X2*'IEA Data'!$E$18</f>
         <v>0.74856543679832355</v>
       </c>
-      <c r="Z2" s="12">
+      <c r="Z2" s="6">
         <f>Y2*'IEA Data'!$E$18</f>
         <v>0.7511884507546045</v>
       </c>
-      <c r="AA2" s="12">
+      <c r="AA2" s="6">
         <f>Z2*'IEA Data'!$E$18</f>
         <v>0.75382065589428315</v>
       </c>
-      <c r="AB2" s="12">
+      <c r="AB2" s="6">
         <f>AA2*'IEA Data'!$E$18</f>
         <v>0.7564620844237655</v>
       </c>
-      <c r="AC2" s="12">
+      <c r="AC2" s="6">
         <f>AB2*'IEA Data'!$E$18</f>
         <v>0.75911276866231048</v>
       </c>
-      <c r="AD2" s="12">
+      <c r="AD2" s="6">
         <f>AC2*'IEA Data'!$E$18</f>
         <v>0.76177274104242554</v>
       </c>
-      <c r="AE2" s="12">
+      <c r="AE2" s="6">
         <f>AD2*'IEA Data'!$E$18</f>
         <v>0.76444203411026324</v>
       </c>
-      <c r="AF2" s="12">
+      <c r="AF2" s="6">
         <f>AE2*'IEA Data'!$E$18</f>
         <v>0.76712068052601967</v>
       </c>
-      <c r="AG2" s="12">
+      <c r="AG2" s="6">
         <f>AF2*'IEA Data'!$E$18</f>
         <v>0.76980871306433407</v>
       </c>
-      <c r="AH2" s="12">
+      <c r="AH2" s="6">
         <f>AG2*'IEA Data'!$E$18</f>
         <v>0.77250616461468979</v>
       </c>
-      <c r="AI2" s="12">
+      <c r="AI2" s="6">
         <f>AH2*'IEA Data'!$E$18</f>
         <v>0.77521306818181679</v>
       </c>
@@ -1247,140 +1258,140 @@
         <v>3</v>
       </c>
       <c r="B3" s="6">
-        <f>118/(162+2+46)</f>
-        <v>0.56190476190476191</v>
+        <f>118/(162+2)</f>
+        <v>0.71951219512195119</v>
       </c>
       <c r="C3" s="6">
         <f>B3</f>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:O3" si="0">C3</f>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="G3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="I3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="K3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="M3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="N3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="O3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="P3" s="13">
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="P3" s="12">
         <f>O3</f>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="Q3" s="12">
-        <f t="shared" ref="Q3:AI3" si="1">P3</f>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="R3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="S3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="T3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="U3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="V3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="W3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="X3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="Y3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="Z3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AA3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AB3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AC3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AD3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AE3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AF3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AG3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AH3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-      <c r="AI3" s="12">
-        <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="Q3" s="6">
+        <f t="shared" ref="Q3:AI6" si="1">P3</f>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="R3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="S3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="T3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="U3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="V3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="W3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="X3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="Y3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="Z3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AA3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AB3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AC3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AD3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AE3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AF3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AG3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AH3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
+      </c>
+      <c r="AI3" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71951219512195119</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
@@ -1443,84 +1454,84 @@
         <f t="shared" si="2"/>
         <v>0.57004830917874394</v>
       </c>
-      <c r="P4" s="13">
-        <f t="shared" si="2"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="Q4" s="12">
-        <f t="shared" ref="Q4:AI4" si="3">P4</f>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="R4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="S4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="T4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="U4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="V4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="W4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="X4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="Y4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="Z4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AA4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AB4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AC4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AD4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AE4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AF4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AG4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AH4" s="12">
-        <f t="shared" si="3"/>
-        <v>0.57004830917874394</v>
-      </c>
-      <c r="AI4" s="12">
-        <f t="shared" si="3"/>
+      <c r="P4" s="12">
+        <f t="shared" si="2"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="Q4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="R4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="S4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="T4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="U4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="V4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="W4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="X4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="Y4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="Z4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AA4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AB4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AC4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AD4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AE4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AF4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AG4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AH4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57004830917874394</v>
+      </c>
+      <c r="AI4" s="6">
+        <f t="shared" si="1"/>
         <v>0.57004830917874394</v>
       </c>
     </row>
@@ -1584,84 +1595,84 @@
         <f t="shared" si="2"/>
         <v>0.46274509803921571</v>
       </c>
-      <c r="P5" s="13">
-        <f t="shared" si="2"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="Q5" s="12">
-        <f t="shared" ref="Q5:AI5" si="4">P5</f>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="R5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="S5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="T5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="U5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="V5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="W5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="X5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="Y5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="Z5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AA5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AB5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AC5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AD5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AE5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AF5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AG5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AH5" s="12">
-        <f t="shared" si="4"/>
-        <v>0.46274509803921571</v>
-      </c>
-      <c r="AI5" s="12">
-        <f t="shared" si="4"/>
+      <c r="P5" s="12">
+        <f t="shared" si="2"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="Q5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="R5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="S5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="T5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="U5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="V5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="W5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="X5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="Z5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AA5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AB5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AC5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AD5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AE5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AF5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AG5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AH5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46274509803921571</v>
+      </c>
+      <c r="AI5" s="6">
+        <f t="shared" si="1"/>
         <v>0.46274509803921571</v>
       </c>
     </row>
@@ -1724,84 +1735,84 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P6" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="12">
-        <f t="shared" ref="Q6:AI6" si="5">P6</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AD6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AG6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AH6" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AI6" s="12">
-        <f t="shared" si="5"/>
+      <c r="P6" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="6">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>